<commit_message>
Set up time slots, need to add conflict constraint
</commit_message>
<xml_diff>
--- a/Testing data.xlsx
+++ b/Testing data.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs 2020 Summer\Timetable DWA\Scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB372DFF-70DD-4A84-979A-4AEC9F9F234A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711B8DD2-0E8C-4464-A5A6-50D10E3986E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6705" yWindow="1605" windowWidth="21600" windowHeight="11265" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CanTeach" sheetId="1" r:id="rId1"/>
     <sheet name="Prefer" sheetId="4" r:id="rId2"/>
     <sheet name="Course" sheetId="2" r:id="rId3"/>
     <sheet name="Prof" sheetId="3" r:id="rId4"/>
+    <sheet name="Time" sheetId="6" r:id="rId5"/>
+    <sheet name="OxyTime" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="41">
   <si>
     <t>Course 1</t>
   </si>
@@ -93,13 +95,79 @@
   </si>
   <si>
     <t>Spring</t>
+  </si>
+  <si>
+    <t>LECTURE PERIODS</t>
+  </si>
+  <si>
+    <t>START TIME</t>
+  </si>
+  <si>
+    <t>END TIME</t>
+  </si>
+  <si>
+    <t>Monday through Friday</t>
+  </si>
+  <si>
+    <t>am</t>
+  </si>
+  <si>
+    <t>pm</t>
+  </si>
+  <si>
+    <t>Monday, Wednesday and Friday</t>
+  </si>
+  <si>
+    <t>Tuesday and Thursday</t>
+  </si>
+  <si>
+    <t>Monday and Wednesday</t>
+  </si>
+  <si>
+    <t>Monday and Friday</t>
+  </si>
+  <si>
+    <t>Wednesday and Friday</t>
+  </si>
+  <si>
+    <t>Tuesday or Thursday</t>
+  </si>
+  <si>
+    <t>Tuesday, Wednesday or Thursday</t>
+  </si>
+  <si>
+    <t>LABORATORY PERIODS</t>
+  </si>
+  <si>
+    <t>Wednesday, or Friday</t>
+  </si>
+  <si>
+    <t>Monday or Wednesday</t>
+  </si>
+  <si>
+    <t>Monday or Wednesday or Thursday</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Thur</t>
+  </si>
+  <si>
+    <t>Fri</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,18 +181,78 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -134,8 +262,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,11 +614,11 @@
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
@@ -473,11 +626,11 @@
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -494,7 +647,7 @@
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
@@ -502,11 +655,11 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
@@ -523,7 +676,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
@@ -535,11 +688,11 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
@@ -572,7 +725,7 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
@@ -585,7 +738,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
@@ -593,7 +746,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
@@ -601,15 +754,15 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -617,32 +770,25 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H7">
-        <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -698,11 +844,11 @@
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
@@ -714,7 +860,7 @@
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -723,11 +869,11 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:H7" ca="1" si="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
@@ -760,23 +906,23 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
@@ -797,11 +943,11 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
@@ -809,7 +955,7 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
@@ -822,15 +968,15 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
@@ -842,11 +988,11 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -863,7 +1009,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
@@ -871,15 +1017,15 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -891,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55087B8-EDE9-4531-8D48-791EBDB20673}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,12 +1069,12 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <f ca="1">RANDBETWEEN(0,2)</f>
-        <v>1</v>
+        <f ca="1">RANDBETWEEN(0,3)</f>
+        <v>0</v>
       </c>
       <c r="E2">
         <f ca="1">ABS(D2-1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -943,7 +1089,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D8" ca="1" si="1">RANDBETWEEN(0,2)</f>
+        <f t="shared" ref="D3:D8" ca="1" si="1">RANDBETWEEN(0,3)</f>
         <v>0</v>
       </c>
       <c r="E3">
@@ -980,15 +1126,15 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <f ca="1">ABS(D5-1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1000,15 +1146,15 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f ca="1">ABS(D6-1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1040,15 +1186,15 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1063,7 +1209,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,4 +1278,1353 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709CA693-7B71-4760-95D6-DBE94D9FE574}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.3923611111111111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0.61805555555555558</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0.3923611111111111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0.4826388888888889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.52777777777777779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0.61805555555555558</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.625</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.66319444444444442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>0</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0.91319444444444453</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>0</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>0</v>
+      </c>
+      <c r="B13" s="10">
+        <v>1</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0.5625</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0.62152777777777779</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>0</v>
+      </c>
+      <c r="B14" s="10">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>0</v>
+      </c>
+      <c r="B15" s="10">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0.76736111111111116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>1</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
+      <c r="C16" s="10">
+        <v>1</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G16" s="11">
+        <v>0.3923611111111111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>1</v>
+      </c>
+      <c r="B17" s="10">
+        <v>0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>1</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>1</v>
+      </c>
+      <c r="B18" s="10">
+        <v>0</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="G18" s="11">
+        <v>0.79513888888888884</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>1</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>1</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0</v>
+      </c>
+      <c r="F19" s="11">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G19" s="11">
+        <v>0.86111111111111116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>1</v>
+      </c>
+      <c r="B20" s="10">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="G20" s="11">
+        <v>0.92708333333333337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>1</v>
+      </c>
+      <c r="B21" s="10">
+        <v>0</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G21" s="11">
+        <v>0.3923611111111111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>1</v>
+      </c>
+      <c r="B22" s="10">
+        <v>0</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1</v>
+      </c>
+      <c r="F22" s="11">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="G22" s="11">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>0</v>
+      </c>
+      <c r="B23" s="10">
+        <v>0</v>
+      </c>
+      <c r="C23" s="10">
+        <v>1</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10">
+        <v>1</v>
+      </c>
+      <c r="F23" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G23" s="11">
+        <v>0.3923611111111111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>0</v>
+      </c>
+      <c r="B24" s="10">
+        <v>0</v>
+      </c>
+      <c r="C24" s="10">
+        <v>1</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+      <c r="E24" s="10">
+        <v>1</v>
+      </c>
+      <c r="F24" s="11">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="G24" s="11">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>0</v>
+      </c>
+      <c r="B25" s="10">
+        <v>1</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0</v>
+      </c>
+      <c r="F25" s="11">
+        <v>0.5625</v>
+      </c>
+      <c r="G25" s="11">
+        <v>0.68402777777777779</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>0</v>
+      </c>
+      <c r="B26" s="10">
+        <v>0</v>
+      </c>
+      <c r="C26" s="10">
+        <v>0</v>
+      </c>
+      <c r="D26" s="10">
+        <v>1</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0</v>
+      </c>
+      <c r="F26" s="11">
+        <v>0.5625</v>
+      </c>
+      <c r="G26" s="11">
+        <v>0.68402777777777779</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>0</v>
+      </c>
+      <c r="B27" s="10">
+        <v>1</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0</v>
+      </c>
+      <c r="F27" s="11">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G27" s="11">
+        <v>0.92708333333333337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>0</v>
+      </c>
+      <c r="B28" s="10">
+        <v>0</v>
+      </c>
+      <c r="C28" s="10">
+        <v>1</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0</v>
+      </c>
+      <c r="F28" s="11">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G28" s="11">
+        <v>0.92708333333333337</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>0</v>
+      </c>
+      <c r="B29" s="10">
+        <v>0</v>
+      </c>
+      <c r="C29" s="10">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10">
+        <v>1</v>
+      </c>
+      <c r="E29" s="10">
+        <v>0</v>
+      </c>
+      <c r="F29" s="11">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G29" s="11">
+        <v>0.92708333333333337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A26F49D5-A316-4571-84F2-F4DF29EA2B57}">
+  <dimension ref="A1:Q34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="32.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="1" customWidth="1"/>
+    <col min="9" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="12.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+    </row>
+    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7">
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.11805555555555557</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.18402777777777779</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+    </row>
+    <row r="4" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="4">
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.20138888888888887</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+    </row>
+    <row r="5" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.4375</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.24652777777777779</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="7">
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.11805555555555557</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="10"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.16319444444444445</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="10"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+    </row>
+    <row r="10" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.17013888888888887</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+    </row>
+    <row r="11" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+    </row>
+    <row r="12" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+    </row>
+    <row r="13" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.12152777777777778</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+    </row>
+    <row r="14" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.1875</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+    </row>
+    <row r="15" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.2673611111111111</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+    </row>
+    <row r="16" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+    </row>
+    <row r="17" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.17013888888888887</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+    </row>
+    <row r="18" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0.23611111111111113</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+    </row>
+    <row r="19" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+    </row>
+    <row r="20" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+    </row>
+    <row r="21" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+    </row>
+    <row r="22" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.17013888888888887</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+    </row>
+    <row r="23" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+    </row>
+    <row r="24" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0.17013888888888887</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+    </row>
+    <row r="25" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.18402777777777779</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+    </row>
+    <row r="26" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+    </row>
+    <row r="28" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+    </row>
+    <row r="29" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+    </row>
+    <row r="30" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Maximize the number of sections offered. Added professors' preference for time slot, using days of the week and time frame during a a day. Maximize the number of time slots professors prefer.
</commit_message>
<xml_diff>
--- a/Testing data.xlsx
+++ b/Testing data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs 2020 Summer\Timetable DWA\Scheduling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs 2020 Summer\department-course-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711B8DD2-0E8C-4464-A5A6-50D10E3986E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD94E1BA-FED7-4765-AD92-36F3594EEC5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6705" yWindow="1605" windowWidth="21600" windowHeight="11265" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12630" yWindow="3000" windowWidth="16170" windowHeight="7365" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CanTeach" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="52">
   <si>
     <t>Course 1</t>
   </si>
@@ -82,9 +82,6 @@
     <t>UnitSum</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
     <t>Course 0</t>
   </si>
   <si>
@@ -161,6 +158,42 @@
   </si>
   <si>
     <t>Fri</t>
+  </si>
+  <si>
+    <t>Afternoon</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>Evening</t>
+  </si>
+  <si>
+    <t>MWF</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>WF</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>MTWRF</t>
   </si>
 </sst>
 </file>
@@ -572,14 +605,14 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -602,15 +635,15 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:H2" ca="1" si="0">MOD(INT(RAND()*100),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
@@ -618,11 +651,11 @@
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
@@ -638,12 +671,12 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:H7" ca="1" si="1">MOD(INT(RAND()*100),2)</f>
+        <f t="shared" ref="B3:H6" ca="1" si="1">MOD(INT(RAND()*100),2)</f>
         <v>1</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
@@ -651,15 +684,15 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
@@ -672,19 +705,19 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
@@ -692,7 +725,7 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
@@ -713,7 +746,7 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
@@ -721,15 +754,15 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -742,7 +775,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
@@ -754,7 +787,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
@@ -762,7 +795,7 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -802,14 +835,14 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -832,7 +865,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
@@ -852,15 +885,15 @@
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -877,11 +910,11 @@
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
@@ -902,15 +935,15 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
@@ -947,7 +980,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
@@ -968,7 +1001,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
@@ -976,23 +1009,23 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1001,11 +1034,11 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
@@ -1025,7 +1058,7 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1037,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55087B8-EDE9-4531-8D48-791EBDB20673}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,15 +1084,15 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -1069,12 +1102,12 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>0</v>
+        <f ca="1">RANDBETWEEN(0,4)</f>
+        <v>1</v>
       </c>
       <c r="E2">
         <f ca="1">ABS(D2-1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,12 +1118,12 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C17" ca="1" si="0">SUM(D3:Y3)*B3</f>
-        <v>4</v>
+        <f t="shared" ref="C3:C8" ca="1" si="0">SUM(D3:Y3)*B3</f>
+        <v>12</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D8" ca="1" si="1">RANDBETWEEN(0,3)</f>
-        <v>0</v>
+        <f t="shared" ref="D3:D8" ca="1" si="1">RANDBETWEEN(0,4)</f>
+        <v>2</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="2">ABS(D3-1)</f>
@@ -1106,15 +1139,15 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1126,15 +1159,15 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <f ca="1">ABS(D5-1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1146,15 +1179,15 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <f ca="1">ABS(D6-1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1186,15 +1219,15 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1206,86 +1239,404 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FE03E8-5E32-411A-8E39-F9A87C02495E}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
         <v>16</v>
       </c>
-      <c r="B2">
-        <v>24</v>
-      </c>
       <c r="C2">
-        <f>SUM(B2:B7)</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <f ca="1">MOD(INT(RAND()*100),2)</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:N2" ca="1" si="0">MOD(INT(RAND()*100),2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:N7" ca="1" si="1">MOD(INT(RAND()*100),2)</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709CA693-7B71-4760-95D6-DBE94D9FE574}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,30 +1645,36 @@
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="F1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1340,7 +1697,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1363,7 +1720,7 @@
         <v>0.61805555555555558</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1386,7 +1743,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1409,7 +1766,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1432,7 +1789,7 @@
         <v>0.4826388888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1455,7 +1812,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1478,7 +1835,7 @@
         <v>0.61805555555555558</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1501,7 +1858,7 @@
         <v>0.66319444444444442</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1524,7 +1881,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>0</v>
       </c>
@@ -1547,7 +1904,7 @@
         <v>0.91319444444444453</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>0</v>
       </c>
@@ -1570,7 +1927,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>0</v>
       </c>
@@ -1593,7 +1950,7 @@
         <v>0.62152777777777779</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>0</v>
       </c>
@@ -1616,7 +1973,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>0</v>
       </c>
@@ -1639,7 +1996,7 @@
         <v>0.76736111111111116</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1962,6 +2319,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1971,7 +2329,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,22 +2349,22 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -2018,7 +2376,7 @@
     </row>
     <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7">
         <v>0.35416666666666669</v>
@@ -2027,10 +2385,10 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="4">
         <v>0.35416666666666669</v>
@@ -2039,7 +2397,7 @@
         <v>0.47569444444444442</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
@@ -2050,7 +2408,7 @@
     </row>
     <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="7">
         <v>7.9861111111111105E-2</v>
@@ -2059,10 +2417,10 @@
         <v>0.11805555555555557</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="4">
         <v>6.25E-2</v>
@@ -2071,7 +2429,7 @@
         <v>0.18402777777777779</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
@@ -2082,7 +2440,7 @@
     </row>
     <row r="4" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="7">
         <v>0.35416666666666669</v>
@@ -2091,10 +2449,10 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="4">
         <v>7.9861111111111105E-2</v>
@@ -2103,7 +2461,7 @@
         <v>0.20138888888888887</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="10"/>
       <c r="P4" s="11"/>
@@ -2111,7 +2469,7 @@
     </row>
     <row r="5" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7">
         <v>0.39930555555555558</v>
@@ -2120,10 +2478,10 @@
         <v>0.4375</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="4">
         <v>0.125</v>
@@ -2132,7 +2490,7 @@
         <v>0.24652777777777779</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L5" s="10"/>
       <c r="P5" s="11"/>
@@ -2140,7 +2498,7 @@
     </row>
     <row r="6" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7">
         <v>0.44444444444444442</v>
@@ -2149,10 +2507,10 @@
         <v>0.4826388888888889</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="4">
         <v>0.30208333333333331</v>
@@ -2161,7 +2519,7 @@
         <v>0.4236111111111111</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L6" s="10"/>
       <c r="P6" s="11"/>
@@ -2169,7 +2527,7 @@
     </row>
     <row r="7" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="8">
         <v>0.48958333333333331</v>
@@ -2178,7 +2536,7 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" s="10"/>
       <c r="P7" s="11"/>
@@ -2186,7 +2544,7 @@
     </row>
     <row r="8" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7">
         <v>7.9861111111111105E-2</v>
@@ -2195,7 +2553,7 @@
         <v>0.11805555555555557</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L8" s="10"/>
       <c r="P8" s="11"/>
@@ -2203,7 +2561,7 @@
     </row>
     <row r="9" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7">
         <v>0.125</v>
@@ -2212,7 +2570,7 @@
         <v>0.16319444444444445</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" s="10"/>
       <c r="P9" s="11"/>
@@ -2220,7 +2578,7 @@
     </row>
     <row r="10" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="7">
         <v>0.17013888888888887</v>
@@ -2229,7 +2587,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L10" s="10"/>
       <c r="P10" s="11"/>
@@ -2237,7 +2595,7 @@
     </row>
     <row r="11" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="7">
         <v>0.35416666666666669</v>
@@ -2246,7 +2604,7 @@
         <v>0.41319444444444442</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
@@ -2258,7 +2616,7 @@
     </row>
     <row r="12" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7">
         <v>0.4201388888888889</v>
@@ -2267,7 +2625,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -2279,7 +2637,7 @@
     </row>
     <row r="13" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="7">
         <v>6.25E-2</v>
@@ -2288,7 +2646,7 @@
         <v>0.12152777777777778</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -2300,7 +2658,7 @@
     </row>
     <row r="14" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="7">
         <v>0.12847222222222224</v>
@@ -2309,7 +2667,7 @@
         <v>0.1875</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -2321,7 +2679,7 @@
     </row>
     <row r="15" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="7">
         <v>0.20833333333333334</v>
@@ -2330,7 +2688,7 @@
         <v>0.2673611111111111</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
@@ -2342,7 +2700,7 @@
     </row>
     <row r="16" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="7">
         <v>0.33333333333333331</v>
@@ -2351,7 +2709,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -2363,7 +2721,7 @@
     </row>
     <row r="17" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="7">
         <v>0.17013888888888887</v>
@@ -2372,7 +2730,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
@@ -2384,7 +2742,7 @@
     </row>
     <row r="18" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="7">
         <v>0.23611111111111113</v>
@@ -2393,7 +2751,7 @@
         <v>0.2951388888888889</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
@@ -2405,7 +2763,7 @@
     </row>
     <row r="19" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="7">
         <v>0.30208333333333331</v>
@@ -2414,7 +2772,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
@@ -2426,7 +2784,7 @@
     </row>
     <row r="20" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="7">
         <v>0.36805555555555558</v>
@@ -2435,7 +2793,7 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
@@ -2447,7 +2805,7 @@
     </row>
     <row r="21" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="7">
         <v>0.33333333333333331</v>
@@ -2456,7 +2814,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
@@ -2468,7 +2826,7 @@
     </row>
     <row r="22" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="7">
         <v>0.17013888888888887</v>
@@ -2477,7 +2835,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
@@ -2489,7 +2847,7 @@
     </row>
     <row r="23" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="7">
         <v>0.33333333333333331</v>
@@ -2498,7 +2856,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
@@ -2510,7 +2868,7 @@
     </row>
     <row r="24" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="7">
         <v>0.17013888888888887</v>
@@ -2519,7 +2877,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
@@ -2531,7 +2889,7 @@
     </row>
     <row r="25" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="7">
         <v>6.25E-2</v>
@@ -2540,7 +2898,7 @@
         <v>0.18402777777777779</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
@@ -2552,7 +2910,7 @@
     </row>
     <row r="26" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="7">
         <v>0.30208333333333331</v>
@@ -2561,7 +2919,7 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>

</xml_diff>

<commit_message>
Added professor timeframe preferences, and assign timetable while maximizing preferences.
</commit_message>
<xml_diff>
--- a/Testing data.xlsx
+++ b/Testing data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs 2020 Summer\Timetable DWA\Scheduling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs 2020 Summer\department-course-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711B8DD2-0E8C-4464-A5A6-50D10E3986E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FB5E7D-7E78-4AF6-9859-84506818250A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6705" yWindow="1605" windowWidth="21600" windowHeight="11265" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CanTeach" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="54">
   <si>
     <t>Course 1</t>
   </si>
@@ -82,9 +82,6 @@
     <t>UnitSum</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
     <t>Course 0</t>
   </si>
   <si>
@@ -161,6 +158,48 @@
   </si>
   <si>
     <t>Fri</t>
+  </si>
+  <si>
+    <t>MWF</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>MTWRF</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>WF</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Morning, Evening</t>
+  </si>
+  <si>
+    <t>Evening</t>
+  </si>
+  <si>
+    <t>Afternoon</t>
+  </si>
+  <si>
+    <t>Morning, Afternoon, Evening</t>
+  </si>
+  <si>
+    <t>Morning</t>
   </si>
 </sst>
 </file>
@@ -579,7 +618,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -602,7 +641,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
@@ -622,11 +661,11 @@
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
@@ -638,16 +677,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:H7" ca="1" si="1">MOD(INT(RAND()*100),2)</f>
+        <f t="shared" ref="B3:H6" ca="1" si="1">MOD(INT(RAND()*100),2)</f>
         <v>1</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
@@ -655,7 +694,7 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
@@ -663,7 +702,7 @@
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -676,7 +715,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
@@ -684,19 +723,19 @@
       </c>
       <c r="E4">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -705,11 +744,11 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
@@ -717,7 +756,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
@@ -725,7 +764,7 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
@@ -754,7 +793,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
@@ -809,7 +848,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -832,11 +871,11 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:H2" ca="1" si="0">MOD(INT(RAND()*100),2)</f>
@@ -844,7 +883,7 @@
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
@@ -852,11 +891,11 @@
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
@@ -877,15 +916,15 @@
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
@@ -893,7 +932,7 @@
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -902,15 +941,15 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
@@ -926,7 +965,7 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -939,7 +978,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
@@ -947,11 +986,11 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
@@ -972,7 +1011,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
@@ -988,7 +1027,7 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
@@ -1001,15 +1040,15 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
@@ -1017,7 +1056,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
@@ -1037,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55087B8-EDE9-4531-8D48-791EBDB20673}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,15 +1090,15 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -1085,16 +1124,16 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C17" ca="1" si="0">SUM(D3:Y3)*B3</f>
+        <f t="shared" ref="C3:C8" ca="1" si="0">SUM(D3:Y3)*B3</f>
         <v>4</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D8" ca="1" si="1">RANDBETWEEN(0,3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="2">ABS(D3-1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1106,15 +1145,15 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1126,11 +1165,11 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f ca="1">ABS(D5-1)</f>
@@ -1146,15 +1185,15 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <f ca="1">ABS(D6-1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1166,11 +1205,11 @@
       </c>
       <c r="C7">
         <f ca="1">SUM(D7:Y7)*B7</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
@@ -1206,72 +1245,164 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FE03E8-5E32-411A-8E39-F9A87C02495E}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
         <v>16</v>
       </c>
-      <c r="B2">
-        <v>24</v>
-      </c>
-      <c r="C2">
-        <f>SUM(B2:B7)</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1284,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709CA693-7B71-4760-95D6-DBE94D9FE574}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,25 +1427,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="F1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1991,22 +2122,22 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -2018,7 +2149,7 @@
     </row>
     <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7">
         <v>0.35416666666666669</v>
@@ -2027,10 +2158,10 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="4">
         <v>0.35416666666666669</v>
@@ -2039,7 +2170,7 @@
         <v>0.47569444444444442</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
@@ -2050,7 +2181,7 @@
     </row>
     <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="7">
         <v>7.9861111111111105E-2</v>
@@ -2059,10 +2190,10 @@
         <v>0.11805555555555557</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="4">
         <v>6.25E-2</v>
@@ -2071,7 +2202,7 @@
         <v>0.18402777777777779</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
@@ -2082,7 +2213,7 @@
     </row>
     <row r="4" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="7">
         <v>0.35416666666666669</v>
@@ -2091,10 +2222,10 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="4">
         <v>7.9861111111111105E-2</v>
@@ -2103,7 +2234,7 @@
         <v>0.20138888888888887</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="10"/>
       <c r="P4" s="11"/>
@@ -2111,7 +2242,7 @@
     </row>
     <row r="5" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7">
         <v>0.39930555555555558</v>
@@ -2120,10 +2251,10 @@
         <v>0.4375</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="4">
         <v>0.125</v>
@@ -2132,7 +2263,7 @@
         <v>0.24652777777777779</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L5" s="10"/>
       <c r="P5" s="11"/>
@@ -2140,7 +2271,7 @@
     </row>
     <row r="6" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7">
         <v>0.44444444444444442</v>
@@ -2149,10 +2280,10 @@
         <v>0.4826388888888889</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="4">
         <v>0.30208333333333331</v>
@@ -2161,7 +2292,7 @@
         <v>0.4236111111111111</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L6" s="10"/>
       <c r="P6" s="11"/>
@@ -2169,7 +2300,7 @@
     </row>
     <row r="7" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="8">
         <v>0.48958333333333331</v>
@@ -2178,7 +2309,7 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" s="10"/>
       <c r="P7" s="11"/>
@@ -2186,7 +2317,7 @@
     </row>
     <row r="8" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7">
         <v>7.9861111111111105E-2</v>
@@ -2195,7 +2326,7 @@
         <v>0.11805555555555557</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L8" s="10"/>
       <c r="P8" s="11"/>
@@ -2203,7 +2334,7 @@
     </row>
     <row r="9" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7">
         <v>0.125</v>
@@ -2212,7 +2343,7 @@
         <v>0.16319444444444445</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" s="10"/>
       <c r="P9" s="11"/>
@@ -2220,7 +2351,7 @@
     </row>
     <row r="10" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="7">
         <v>0.17013888888888887</v>
@@ -2229,7 +2360,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L10" s="10"/>
       <c r="P10" s="11"/>
@@ -2237,7 +2368,7 @@
     </row>
     <row r="11" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="7">
         <v>0.35416666666666669</v>
@@ -2246,7 +2377,7 @@
         <v>0.41319444444444442</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
@@ -2258,7 +2389,7 @@
     </row>
     <row r="12" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7">
         <v>0.4201388888888889</v>
@@ -2267,7 +2398,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -2279,7 +2410,7 @@
     </row>
     <row r="13" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="7">
         <v>6.25E-2</v>
@@ -2288,7 +2419,7 @@
         <v>0.12152777777777778</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -2300,7 +2431,7 @@
     </row>
     <row r="14" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="7">
         <v>0.12847222222222224</v>
@@ -2309,7 +2440,7 @@
         <v>0.1875</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -2321,7 +2452,7 @@
     </row>
     <row r="15" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="7">
         <v>0.20833333333333334</v>
@@ -2330,7 +2461,7 @@
         <v>0.2673611111111111</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
@@ -2342,7 +2473,7 @@
     </row>
     <row r="16" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="7">
         <v>0.33333333333333331</v>
@@ -2351,7 +2482,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -2363,7 +2494,7 @@
     </row>
     <row r="17" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="7">
         <v>0.17013888888888887</v>
@@ -2372,7 +2503,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
@@ -2384,7 +2515,7 @@
     </row>
     <row r="18" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="7">
         <v>0.23611111111111113</v>
@@ -2393,7 +2524,7 @@
         <v>0.2951388888888889</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
@@ -2405,7 +2536,7 @@
     </row>
     <row r="19" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="7">
         <v>0.30208333333333331</v>
@@ -2414,7 +2545,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
@@ -2426,7 +2557,7 @@
     </row>
     <row r="20" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="7">
         <v>0.36805555555555558</v>
@@ -2435,7 +2566,7 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
@@ -2447,7 +2578,7 @@
     </row>
     <row r="21" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="7">
         <v>0.33333333333333331</v>
@@ -2456,7 +2587,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
@@ -2468,7 +2599,7 @@
     </row>
     <row r="22" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="7">
         <v>0.17013888888888887</v>
@@ -2477,7 +2608,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
@@ -2489,7 +2620,7 @@
     </row>
     <row r="23" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="7">
         <v>0.33333333333333331</v>
@@ -2498,7 +2629,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
@@ -2510,7 +2641,7 @@
     </row>
     <row r="24" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="7">
         <v>0.17013888888888887</v>
@@ -2519,7 +2650,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
@@ -2531,7 +2662,7 @@
     </row>
     <row r="25" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="7">
         <v>6.25E-2</v>
@@ -2540,7 +2671,7 @@
         <v>0.18402777777777779</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
@@ -2552,7 +2683,7 @@
     </row>
     <row r="26" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="7">
         <v>0.30208333333333331</v>
@@ -2561,7 +2692,7 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>

</xml_diff>

<commit_message>
cleaned loops in prof time conflict.
</commit_message>
<xml_diff>
--- a/Testing data.xlsx
+++ b/Testing data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs 2020 Summer\department-course-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FB5E7D-7E78-4AF6-9859-84506818250A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3070E87C-99EA-44DE-A15C-52985AB60680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CanTeach" sheetId="1" r:id="rId1"/>
@@ -645,7 +645,7 @@
       </c>
       <c r="B2">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:H2" ca="1" si="0">MOD(INT(RAND()*100),2)</f>
@@ -657,19 +657,19 @@
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -682,15 +682,15 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -711,7 +711,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
@@ -719,23 +719,23 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
@@ -781,11 +781,11 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
@@ -793,15 +793,15 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCE1BA5-4E35-4BCB-B104-2CE874789A6D}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
@@ -883,11 +883,11 @@
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
@@ -895,11 +895,11 @@
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -920,7 +920,7 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
@@ -928,11 +928,11 @@
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -953,11 +953,11 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
@@ -974,19 +974,19 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
@@ -1007,11 +1007,11 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
@@ -1019,15 +1019,15 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
@@ -1040,11 +1040,11 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
@@ -1052,19 +1052,19 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1105,11 +1105,11 @@
       </c>
       <c r="C2">
         <f ca="1">SUM(D2:Y2)*B2</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <f ca="1">ABS(D2-1)</f>
@@ -1125,15 +1125,15 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">SUM(D3:Y3)*B3</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D8" ca="1" si="1">RANDBETWEEN(0,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="2">ABS(D3-1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1145,15 +1145,15 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1165,15 +1165,15 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <f ca="1">ABS(D5-1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1185,15 +1185,15 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f ca="1">ABS(D6-1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1205,15 +1205,15 @@
       </c>
       <c r="C7">
         <f ca="1">SUM(D7:Y7)*B7</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,15 +1225,15 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1415,7 +1415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709CA693-7B71-4760-95D6-DBE94D9FE574}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
A course is either optional or must be offered.
</commit_message>
<xml_diff>
--- a/Testing data.xlsx
+++ b/Testing data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs 2020 Summer\department-course-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3070E87C-99EA-44DE-A15C-52985AB60680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FD9BC5-9442-4033-962D-FEE1BF3AF008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14970" yWindow="6720" windowWidth="12645" windowHeight="7365" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CanTeach" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>MaxUnit</t>
   </si>
   <si>
-    <t>UnitSum</t>
-  </si>
-  <si>
     <t>Course 0</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>Morning</t>
+  </si>
+  <si>
+    <t>Must Offer</t>
   </si>
 </sst>
 </file>
@@ -611,14 +611,14 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -641,11 +641,11 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:H2" ca="1" si="0">MOD(INT(RAND()*100),2)</f>
@@ -665,7 +665,7 @@
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
@@ -686,7 +686,7 @@
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -731,11 +731,11 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -744,11 +744,11 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
@@ -760,11 +760,11 @@
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
@@ -777,23 +777,23 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
@@ -801,7 +801,7 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -840,15 +840,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCE1BA5-4E35-4BCB-B104-2CE874789A6D}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -871,15 +871,15 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:H2" ca="1" si="0">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
@@ -887,7 +887,7 @@
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
@@ -899,7 +899,7 @@
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -916,11 +916,11 @@
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
@@ -932,7 +932,7 @@
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
@@ -953,15 +953,15 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
@@ -978,15 +978,15 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
@@ -994,11 +994,11 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1007,23 +1007,23 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
@@ -1076,36 +1076,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55087B8-EDE9-4531-8D48-791EBDB20673}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
       <c r="C2">
-        <f ca="1">SUM(D2:Y2)*B2</f>
-        <v>24</v>
+        <f ca="1">MOD(INT(RAND()*100),2)</f>
+        <v>1</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(0,3)</f>
@@ -1124,12 +1127,12 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C8" ca="1" si="0">SUM(D3:Y3)*B3</f>
-        <v>12</v>
+        <f t="shared" ref="C3:C8" ca="1" si="0">MOD(INT(RAND()*100),2)</f>
+        <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D8" ca="1" si="1">RANDBETWEEN(0,3)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="2">ABS(D3-1)</f>
@@ -1144,16 +1147,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <f ca="1">MOD(INT(RAND()*100),2)</f>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1165,7 +1168,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
@@ -1185,7 +1188,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
@@ -1204,8 +1207,8 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <f ca="1">SUM(D7:Y7)*B7</f>
-        <v>20</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
@@ -1225,7 +1228,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
@@ -1261,51 +1264,51 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>47</v>
-      </c>
-      <c r="K1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>16</v>
       </c>
       <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" t="s">
-        <v>50</v>
-      </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1316,13 +1319,13 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
         <v>51</v>
-      </c>
-      <c r="H3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1333,16 +1336,16 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" t="s">
         <v>51</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1353,16 +1356,16 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
         <v>51</v>
       </c>
-      <c r="F5" t="s">
-        <v>52</v>
-      </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1373,13 +1376,13 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" t="s">
         <v>52</v>
-      </c>
-      <c r="H6" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1390,19 +1393,19 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
         <v>49</v>
       </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>50</v>
       </c>
-      <c r="I7" t="s">
-        <v>51</v>
-      </c>
       <c r="K7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1427,25 +1430,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>39</v>
-      </c>
       <c r="F1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2122,22 +2125,22 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -2149,7 +2152,7 @@
     </row>
     <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="7">
         <v>0.35416666666666669</v>
@@ -2158,10 +2161,10 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="4">
         <v>0.35416666666666669</v>
@@ -2170,7 +2173,7 @@
         <v>0.47569444444444442</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
@@ -2181,7 +2184,7 @@
     </row>
     <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="7">
         <v>7.9861111111111105E-2</v>
@@ -2190,10 +2193,10 @@
         <v>0.11805555555555557</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="4">
         <v>6.25E-2</v>
@@ -2202,7 +2205,7 @@
         <v>0.18402777777777779</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
@@ -2213,7 +2216,7 @@
     </row>
     <row r="4" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="7">
         <v>0.35416666666666669</v>
@@ -2222,10 +2225,10 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="4">
         <v>7.9861111111111105E-2</v>
@@ -2234,7 +2237,7 @@
         <v>0.20138888888888887</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="10"/>
       <c r="P4" s="11"/>
@@ -2242,7 +2245,7 @@
     </row>
     <row r="5" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="7">
         <v>0.39930555555555558</v>
@@ -2251,10 +2254,10 @@
         <v>0.4375</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="4">
         <v>0.125</v>
@@ -2263,7 +2266,7 @@
         <v>0.24652777777777779</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L5" s="10"/>
       <c r="P5" s="11"/>
@@ -2271,7 +2274,7 @@
     </row>
     <row r="6" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="7">
         <v>0.44444444444444442</v>
@@ -2280,10 +2283,10 @@
         <v>0.4826388888888889</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="4">
         <v>0.30208333333333331</v>
@@ -2292,7 +2295,7 @@
         <v>0.4236111111111111</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L6" s="10"/>
       <c r="P6" s="11"/>
@@ -2300,7 +2303,7 @@
     </row>
     <row r="7" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="8">
         <v>0.48958333333333331</v>
@@ -2309,7 +2312,7 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L7" s="10"/>
       <c r="P7" s="11"/>
@@ -2317,7 +2320,7 @@
     </row>
     <row r="8" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="7">
         <v>7.9861111111111105E-2</v>
@@ -2326,7 +2329,7 @@
         <v>0.11805555555555557</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L8" s="10"/>
       <c r="P8" s="11"/>
@@ -2334,7 +2337,7 @@
     </row>
     <row r="9" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="7">
         <v>0.125</v>
@@ -2343,7 +2346,7 @@
         <v>0.16319444444444445</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" s="10"/>
       <c r="P9" s="11"/>
@@ -2351,7 +2354,7 @@
     </row>
     <row r="10" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="7">
         <v>0.17013888888888887</v>
@@ -2360,7 +2363,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L10" s="10"/>
       <c r="P10" s="11"/>
@@ -2368,7 +2371,7 @@
     </row>
     <row r="11" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="7">
         <v>0.35416666666666669</v>
@@ -2377,7 +2380,7 @@
         <v>0.41319444444444442</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
@@ -2389,7 +2392,7 @@
     </row>
     <row r="12" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="7">
         <v>0.4201388888888889</v>
@@ -2398,7 +2401,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -2410,7 +2413,7 @@
     </row>
     <row r="13" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="7">
         <v>6.25E-2</v>
@@ -2419,7 +2422,7 @@
         <v>0.12152777777777778</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -2431,7 +2434,7 @@
     </row>
     <row r="14" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="7">
         <v>0.12847222222222224</v>
@@ -2440,7 +2443,7 @@
         <v>0.1875</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -2452,7 +2455,7 @@
     </row>
     <row r="15" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="7">
         <v>0.20833333333333334</v>
@@ -2461,7 +2464,7 @@
         <v>0.2673611111111111</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
@@ -2473,7 +2476,7 @@
     </row>
     <row r="16" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="7">
         <v>0.33333333333333331</v>
@@ -2482,7 +2485,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -2494,7 +2497,7 @@
     </row>
     <row r="17" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="7">
         <v>0.17013888888888887</v>
@@ -2503,7 +2506,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
@@ -2515,7 +2518,7 @@
     </row>
     <row r="18" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="7">
         <v>0.23611111111111113</v>
@@ -2524,7 +2527,7 @@
         <v>0.2951388888888889</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
@@ -2536,7 +2539,7 @@
     </row>
     <row r="19" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="7">
         <v>0.30208333333333331</v>
@@ -2545,7 +2548,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
@@ -2557,7 +2560,7 @@
     </row>
     <row r="20" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="7">
         <v>0.36805555555555558</v>
@@ -2566,7 +2569,7 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
@@ -2578,7 +2581,7 @@
     </row>
     <row r="21" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="7">
         <v>0.33333333333333331</v>
@@ -2587,7 +2590,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
@@ -2599,7 +2602,7 @@
     </row>
     <row r="22" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="7">
         <v>0.17013888888888887</v>
@@ -2608,7 +2611,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
@@ -2620,7 +2623,7 @@
     </row>
     <row r="23" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="7">
         <v>0.33333333333333331</v>
@@ -2629,7 +2632,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
@@ -2641,7 +2644,7 @@
     </row>
     <row r="24" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="7">
         <v>0.17013888888888887</v>
@@ -2650,7 +2653,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
@@ -2662,7 +2665,7 @@
     </row>
     <row r="25" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="7">
         <v>6.25E-2</v>
@@ -2671,7 +2674,7 @@
         <v>0.18402777777777779</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
@@ -2683,7 +2686,7 @@
     </row>
     <row r="26" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="7">
         <v>0.30208333333333331</v>
@@ -2692,7 +2695,7 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>

</xml_diff>

<commit_message>
Changed must_offer from booleans to int for each semester
</commit_message>
<xml_diff>
--- a/Testing data.xlsx
+++ b/Testing data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs 2020 Summer\department-course-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FD9BC5-9442-4033-962D-FEE1BF3AF008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BCCA46-0254-4437-89B4-887573041B51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14970" yWindow="6720" windowWidth="12645" windowHeight="7365" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CanTeach" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="55">
   <si>
     <t>Course 1</t>
   </si>
@@ -199,7 +199,10 @@
     <t>Morning</t>
   </si>
   <si>
-    <t>Must Offer</t>
+    <t>Fall_MustOffer</t>
+  </si>
+  <si>
+    <t>Spring_MustOffer</t>
   </si>
 </sst>
 </file>
@@ -614,9 +617,9 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -639,7 +642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -665,14 +668,14 @@
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -682,7 +685,7 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
@@ -694,18 +697,18 @@
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -715,7 +718,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
@@ -723,7 +726,7 @@
       </c>
       <c r="E4">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
@@ -731,14 +734,14 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -748,11 +751,11 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
@@ -764,14 +767,14 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -781,11 +784,11 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
@@ -793,18 +796,18 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -844,9 +847,9 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -869,21 +872,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:H2" ca="1" si="0">MOD(INT(RAND()*100),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
@@ -895,20 +898,20 @@
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:H7" ca="1" si="1">MOD(INT(RAND()*100),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
@@ -916,7 +919,7 @@
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
@@ -932,10 +935,10 @@
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -945,15 +948,15 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
@@ -961,14 +964,14 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -982,7 +985,7 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
@@ -998,20 +1001,20 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
@@ -1019,7 +1022,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
@@ -1031,16 +1034,16 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
@@ -1048,15 +1051,15 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
@@ -1064,7 +1067,7 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1074,32 +1077,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55087B8-EDE9-4531-8D48-791EBDB20673}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1107,19 +1114,23 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <f ca="1">MOD(INT(RAND()*100),2)</f>
+        <f ca="1">RANDBETWEEN(0,3)</f>
         <v>1</v>
       </c>
       <c r="D2">
-        <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>2</v>
+        <f ca="1">RANDBETWEEN(0,C2)</f>
+        <v>1</v>
       </c>
       <c r="E2">
-        <f ca="1">ABS(D2-1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <f ca="1">ABS(C2-1)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f ca="1">RANDBETWEEN(0,E2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1127,19 +1138,23 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C8" ca="1" si="0">MOD(INT(RAND()*100),2)</f>
+        <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(0,3)</f>
         <v>1</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D8" ca="1" si="1">RANDBETWEEN(0,3)</f>
-        <v>0</v>
+        <f t="shared" ref="D3:D8" ca="1" si="1">RANDBETWEEN(0,C3)</f>
+        <v>1</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E8" ca="1" si="2">ABS(D3-1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E3:E8" ca="1" si="2">ABS(C3-1)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f ca="1">RANDBETWEEN(0,E3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1147,19 +1162,23 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F3:F8" ca="1" si="3">RANDBETWEEN(0,E4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1172,14 +1191,18 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <f ca="1">ABS(D5-1)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1188,18 +1211,22 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="E6">
-        <f ca="1">ABS(D6-1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1208,18 +1235,22 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1237,6 +1268,10 @@
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
         <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1254,12 +1289,12 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -1291,7 +1326,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1311,7 +1346,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1328,7 +1363,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1348,7 +1383,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1368,7 +1403,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1385,7 +1420,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1422,13 +1457,13 @@
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>34</v>
       </c>
@@ -1451,7 +1486,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1474,7 +1509,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1497,7 +1532,7 @@
         <v>0.61805555555555558</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1520,7 +1555,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1543,7 +1578,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1566,7 +1601,7 @@
         <v>0.4826388888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1589,7 +1624,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1612,7 +1647,7 @@
         <v>0.61805555555555558</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1635,7 +1670,7 @@
         <v>0.66319444444444442</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1658,7 +1693,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>0</v>
       </c>
@@ -1681,7 +1716,7 @@
         <v>0.91319444444444453</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>0</v>
       </c>
@@ -1704,7 +1739,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>0</v>
       </c>
@@ -1727,7 +1762,7 @@
         <v>0.62152777777777779</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>0</v>
       </c>
@@ -1750,7 +1785,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>0</v>
       </c>
@@ -1773,7 +1808,7 @@
         <v>0.76736111111111116</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1796,7 +1831,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>1</v>
       </c>
@@ -1819,7 +1854,7 @@
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>1</v>
       </c>
@@ -1842,7 +1877,7 @@
         <v>0.79513888888888884</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>1</v>
       </c>
@@ -1865,7 +1900,7 @@
         <v>0.86111111111111116</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>1</v>
       </c>
@@ -1888,7 +1923,7 @@
         <v>0.92708333333333337</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>1</v>
       </c>
@@ -1911,7 +1946,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <v>1</v>
       </c>
@@ -1934,7 +1969,7 @@
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <v>0</v>
       </c>
@@ -1957,7 +1992,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>0</v>
       </c>
@@ -1980,7 +2015,7 @@
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
         <v>0</v>
       </c>
@@ -2003,7 +2038,7 @@
         <v>0.68402777777777779</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <v>0</v>
       </c>
@@ -2026,7 +2061,7 @@
         <v>0.68402777777777779</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <v>0</v>
       </c>
@@ -2049,7 +2084,7 @@
         <v>0.92708333333333337</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
         <v>0</v>
       </c>
@@ -2072,7 +2107,7 @@
         <v>0.92708333333333337</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
         <v>0</v>
       </c>
@@ -2108,22 +2143,22 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="32.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" customWidth="1"/>
-    <col min="9" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="12.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="32.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1"/>
+    <col min="6" max="6" width="32.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" style="1" customWidth="1"/>
+    <col min="9" max="15" width="9.1796875" style="1"/>
+    <col min="16" max="16" width="12.1796875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7265625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -2150,7 +2185,7 @@
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
     </row>
-    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -2182,7 +2217,7 @@
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2214,7 +2249,7 @@
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
     </row>
-    <row r="4" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -2243,7 +2278,7 @@
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
     </row>
-    <row r="5" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -2272,7 +2307,7 @@
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
     </row>
-    <row r="6" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2301,7 +2336,7 @@
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
     </row>
-    <row r="7" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -2318,7 +2353,7 @@
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
     </row>
-    <row r="8" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -2335,7 +2370,7 @@
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
     </row>
-    <row r="9" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -2352,7 +2387,7 @@
       <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
     </row>
-    <row r="10" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -2369,7 +2404,7 @@
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
     </row>
-    <row r="11" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -2390,7 +2425,7 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
     </row>
-    <row r="12" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -2411,7 +2446,7 @@
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
     </row>
-    <row r="13" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -2432,7 +2467,7 @@
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
     </row>
-    <row r="14" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -2453,7 +2488,7 @@
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
     </row>
-    <row r="15" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -2474,7 +2509,7 @@
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
     </row>
-    <row r="16" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -2495,7 +2530,7 @@
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
     </row>
-    <row r="17" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -2516,7 +2551,7 @@
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
     </row>
-    <row r="18" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -2537,7 +2572,7 @@
       <c r="P18" s="11"/>
       <c r="Q18" s="11"/>
     </row>
-    <row r="19" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2558,7 +2593,7 @@
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
     </row>
-    <row r="20" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -2579,7 +2614,7 @@
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
     </row>
-    <row r="21" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -2600,7 +2635,7 @@
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
     </row>
-    <row r="22" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -2621,7 +2656,7 @@
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
     </row>
-    <row r="23" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -2642,7 +2677,7 @@
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
     </row>
-    <row r="24" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -2663,7 +2698,7 @@
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
     </row>
-    <row r="25" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -2684,7 +2719,7 @@
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
     </row>
-    <row r="26" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -2705,7 +2740,7 @@
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="K27" s="10"/>
@@ -2716,7 +2751,7 @@
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
     </row>
-    <row r="28" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="17.5" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="K28" s="10"/>
@@ -2727,7 +2762,7 @@
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
     </row>
-    <row r="29" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="K29" s="10"/>
@@ -2738,23 +2773,23 @@
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
     </row>
-    <row r="30" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a method that read input from a excel file.
</commit_message>
<xml_diff>
--- a/Testing data.xlsx
+++ b/Testing data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs 2020 Summer\department-course-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BCCA46-0254-4437-89B4-887573041B51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53427629-1E1C-402F-B200-C252115DBEEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CanTeach" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="86">
   <si>
     <t>Course 1</t>
   </si>
@@ -203,6 +203,99 @@
   </si>
   <si>
     <t>Spring_MustOffer</t>
+  </si>
+  <si>
+    <t>08:30:00</t>
+  </si>
+  <si>
+    <t>13:55:00</t>
+  </si>
+  <si>
+    <t>09:35:00</t>
+  </si>
+  <si>
+    <t>10:40:00</t>
+  </si>
+  <si>
+    <t>11:45:00</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>16:05:00</t>
+  </si>
+  <si>
+    <t>10:05:00</t>
+  </si>
+  <si>
+    <t>13:30:00</t>
+  </si>
+  <si>
+    <t>15:05:00</t>
+  </si>
+  <si>
+    <t>17:00:00</t>
+  </si>
+  <si>
+    <t>08:00:00</t>
+  </si>
+  <si>
+    <t>17:40:00</t>
+  </si>
+  <si>
+    <t>19:15:00</t>
+  </si>
+  <si>
+    <t>20:50:00</t>
+  </si>
+  <si>
+    <t>09:25:00</t>
+  </si>
+  <si>
+    <t>14:50:00</t>
+  </si>
+  <si>
+    <t>10:30:00</t>
+  </si>
+  <si>
+    <t>11:35:00</t>
+  </si>
+  <si>
+    <t>12:40:00</t>
+  </si>
+  <si>
+    <t>15:55:00</t>
+  </si>
+  <si>
+    <t>21:55:00</t>
+  </si>
+  <si>
+    <t>11:30:00</t>
+  </si>
+  <si>
+    <t>14:55:00</t>
+  </si>
+  <si>
+    <t>16:30:00</t>
+  </si>
+  <si>
+    <t>18:25:00</t>
+  </si>
+  <si>
+    <t>17:30:00</t>
+  </si>
+  <si>
+    <t>19:05:00</t>
+  </si>
+  <si>
+    <t>20:40:00</t>
+  </si>
+  <si>
+    <t>22:15:00</t>
+  </si>
+  <si>
+    <t>16:25:00</t>
   </si>
 </sst>
 </file>
@@ -652,11 +745,11 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:H2" ca="1" si="0">MOD(INT(RAND()*100),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
@@ -664,7 +757,7 @@
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
@@ -672,7 +765,7 @@
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -685,19 +778,19 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
@@ -722,7 +815,7 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
@@ -738,7 +831,7 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -747,7 +840,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
@@ -759,11 +852,11 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
@@ -771,7 +864,7 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -788,19 +881,19 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f ca="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
@@ -890,19 +983,19 @@
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -911,31 +1004,31 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:H7" ca="1" si="1">MOD(INT(RAND()*100),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -952,15 +1045,15 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
@@ -968,7 +1061,7 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -977,7 +1070,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
@@ -997,11 +1090,11 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1014,7 +1107,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
@@ -1030,11 +1123,11 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1055,11 +1148,11 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
@@ -1067,7 +1160,7 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1079,7 +1172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55087B8-EDE9-4531-8D48-791EBDB20673}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -1119,7 +1212,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(0,C2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f ca="1">ABS(C2-1)</f>
@@ -1139,15 +1232,15 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C8" ca="1" si="0">RANDBETWEEN(0,3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D8" ca="1" si="1">RANDBETWEEN(0,C3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" ca="1" si="2">ABS(C3-1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <f ca="1">RANDBETWEEN(0,E3)</f>
@@ -1163,19 +1256,19 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F3:F8" ca="1" si="3">RANDBETWEEN(0,E4)</f>
-        <v>2</v>
+        <f t="shared" ref="F4:F8" ca="1" si="3">RANDBETWEEN(0,E4)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1235,15 +1328,15 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="3"/>
@@ -1259,7 +1352,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
@@ -1453,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709CA693-7B71-4760-95D6-DBE94D9FE574}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1502,11 +1595,11 @@
       <c r="E2" s="10">
         <v>1</v>
       </c>
-      <c r="F2" s="11">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="G2" s="11">
-        <v>0.3923611111111111</v>
+      <c r="F2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1525,11 +1618,11 @@
       <c r="E3" s="10">
         <v>1</v>
       </c>
-      <c r="F3" s="11">
-        <v>0.57986111111111105</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0.61805555555555558</v>
+      <c r="F3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1548,11 +1641,11 @@
       <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="11">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="G4" s="11">
-        <v>0.3923611111111111</v>
+      <c r="F4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1571,11 +1664,11 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="11">
-        <v>0.39930555555555558</v>
-      </c>
-      <c r="G5" s="11">
-        <v>0.4375</v>
+      <c r="F5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -1594,11 +1687,11 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="11">
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="G6" s="11">
-        <v>0.4826388888888889</v>
+      <c r="F6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -1617,11 +1710,11 @@
       <c r="E7" s="1">
         <v>1</v>
       </c>
-      <c r="F7" s="11">
-        <v>0.48958333333333331</v>
-      </c>
-      <c r="G7" s="11">
-        <v>0.52777777777777779</v>
+      <c r="F7" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1640,11 +1733,11 @@
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="11">
-        <v>0.57986111111111105</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0.61805555555555558</v>
+      <c r="F8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -1663,11 +1756,11 @@
       <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="F9" s="11">
-        <v>0.625</v>
-      </c>
-      <c r="G9" s="11">
-        <v>0.66319444444444442</v>
+      <c r="F9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -1686,11 +1779,11 @@
       <c r="E10" s="1">
         <v>1</v>
       </c>
-      <c r="F10" s="11">
-        <v>0.67013888888888884</v>
-      </c>
-      <c r="G10" s="11">
-        <v>0.70833333333333337</v>
+      <c r="F10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -1709,11 +1802,11 @@
       <c r="E11" s="10">
         <v>0</v>
       </c>
-      <c r="F11" s="11">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="G11" s="11">
-        <v>0.91319444444444453</v>
+      <c r="F11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1732,11 +1825,11 @@
       <c r="E12" s="10">
         <v>0</v>
       </c>
-      <c r="F12" s="11">
-        <v>0.4201388888888889</v>
-      </c>
-      <c r="G12" s="11">
-        <v>0.47916666666666669</v>
+      <c r="F12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1755,11 +1848,11 @@
       <c r="E13" s="10">
         <v>0</v>
       </c>
-      <c r="F13" s="11">
-        <v>0.5625</v>
-      </c>
-      <c r="G13" s="11">
-        <v>0.62152777777777779</v>
+      <c r="F13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1778,11 +1871,11 @@
       <c r="E14" s="10">
         <v>0</v>
       </c>
-      <c r="F14" s="11">
-        <v>0.62847222222222221</v>
-      </c>
-      <c r="G14" s="11">
-        <v>0.6875</v>
+      <c r="F14" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1801,11 +1894,11 @@
       <c r="E15" s="10">
         <v>0</v>
       </c>
-      <c r="F15" s="11">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="G15" s="11">
-        <v>0.76736111111111116</v>
+      <c r="F15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -1824,11 +1917,11 @@
       <c r="E16" s="10">
         <v>0</v>
       </c>
-      <c r="F16" s="11">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G16" s="11">
-        <v>0.3923611111111111</v>
+      <c r="F16" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1847,11 +1940,11 @@
       <c r="E17" s="10">
         <v>0</v>
       </c>
-      <c r="F17" s="11">
-        <v>0.67013888888888884</v>
-      </c>
-      <c r="G17" s="11">
-        <v>0.72916666666666663</v>
+      <c r="F17" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1870,11 +1963,11 @@
       <c r="E18" s="10">
         <v>0</v>
       </c>
-      <c r="F18" s="11">
-        <v>0.73611111111111116</v>
-      </c>
-      <c r="G18" s="11">
-        <v>0.79513888888888884</v>
+      <c r="F18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1893,11 +1986,11 @@
       <c r="E19" s="10">
         <v>0</v>
       </c>
-      <c r="F19" s="11">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="G19" s="11">
-        <v>0.86111111111111116</v>
+      <c r="F19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1916,11 +2009,11 @@
       <c r="E20" s="10">
         <v>0</v>
       </c>
-      <c r="F20" s="11">
-        <v>0.86805555555555547</v>
-      </c>
-      <c r="G20" s="11">
-        <v>0.92708333333333337</v>
+      <c r="F20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1939,11 +2032,11 @@
       <c r="E21" s="10">
         <v>1</v>
       </c>
-      <c r="F21" s="11">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G21" s="11">
-        <v>0.3923611111111111</v>
+      <c r="F21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1962,11 +2055,11 @@
       <c r="E22" s="10">
         <v>1</v>
       </c>
-      <c r="F22" s="11">
-        <v>0.67013888888888884</v>
-      </c>
-      <c r="G22" s="11">
-        <v>0.72916666666666663</v>
+      <c r="F22" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1985,11 +2078,11 @@
       <c r="E23" s="10">
         <v>1</v>
       </c>
-      <c r="F23" s="11">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G23" s="11">
-        <v>0.3923611111111111</v>
+      <c r="F23" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -2008,11 +2101,11 @@
       <c r="E24" s="10">
         <v>1</v>
       </c>
-      <c r="F24" s="11">
-        <v>0.67013888888888884</v>
-      </c>
-      <c r="G24" s="11">
-        <v>0.72916666666666663</v>
+      <c r="F24" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -2031,11 +2124,11 @@
       <c r="E25" s="10">
         <v>0</v>
       </c>
-      <c r="F25" s="11">
-        <v>0.5625</v>
-      </c>
-      <c r="G25" s="11">
-        <v>0.68402777777777779</v>
+      <c r="F25" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -2054,11 +2147,11 @@
       <c r="E26" s="10">
         <v>0</v>
       </c>
-      <c r="F26" s="11">
-        <v>0.5625</v>
-      </c>
-      <c r="G26" s="11">
-        <v>0.68402777777777779</v>
+      <c r="F26" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -2077,11 +2170,11 @@
       <c r="E27" s="10">
         <v>0</v>
       </c>
-      <c r="F27" s="11">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="G27" s="11">
-        <v>0.92708333333333337</v>
+      <c r="F27" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -2100,11 +2193,11 @@
       <c r="E28" s="10">
         <v>0</v>
       </c>
-      <c r="F28" s="11">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="G28" s="11">
-        <v>0.92708333333333337</v>
+      <c r="F28" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -2123,11 +2216,11 @@
       <c r="E29" s="10">
         <v>0</v>
       </c>
-      <c r="F29" s="11">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="G29" s="11">
-        <v>0.92708333333333337</v>
+      <c r="F29" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>